<commit_message>
Added calculated columns, added fieldNumber column
</commit_message>
<xml_diff>
--- a/GGI Barcoding Specimen Spreadsheet.xlsx
+++ b/GGI Barcoding Specimen Spreadsheet.xlsx
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>extractionPlateID</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>projectID</t>
+  </si>
+  <si>
+    <t>fieldNumber</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,6 +478,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor rgb="FF6D9EEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -488,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -500,6 +527,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE95"/>
+  <dimension ref="A1:AF97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -820,20 +852,21 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
     <col min="11" max="11" width="16.109375" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
     <col min="13" max="13" width="9.44140625" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" customWidth="1"/>
     <col min="15" max="15" width="19.5546875" customWidth="1"/>
     <col min="17" max="17" width="17.88671875" customWidth="1"/>
-    <col min="30" max="30" width="13.88671875" customWidth="1"/>
-    <col min="31" max="31" width="20.5546875" customWidth="1"/>
+    <col min="30" max="30" width="14.44140625" style="12"/>
+    <col min="31" max="31" width="13.88671875" customWidth="1"/>
+    <col min="32" max="32" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>124</v>
       </c>
@@ -853,16 +886,16 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>9</v>
@@ -892,511 +925,1650 @@
         <v>17</v>
       </c>
       <c r="T1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="10" t="str">
+        <f>G2&amp;":"&amp;H2&amp;":"&amp;I2</f>
+        <v>::</v>
+      </c>
+      <c r="AE2" s="10" t="str">
+        <f>L2&amp;": "&amp;M2</f>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF2" s="10" t="str">
+        <f>TEXT(R2,"dd-")&amp;TEXT(Q2,"mmm-")&amp;TEXT(P2, "yyyy")</f>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="10" t="str">
+        <f t="shared" ref="J3:J66" si="0">G3&amp;":"&amp;H3&amp;":"&amp;I3</f>
+        <v>::</v>
+      </c>
+      <c r="AE3" s="10" t="str">
+        <f t="shared" ref="AE3:AE66" si="1">L3&amp;": "&amp;M3</f>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF3" s="10" t="str">
+        <f t="shared" ref="AF3:AF66" si="2">TEXT(R3,"dd-")&amp;TEXT(Q3,"mmm-")&amp;TEXT(P3, "yyyy")</f>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF4" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE5" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF5" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE6" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF6" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE7" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF7" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF8" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE9" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF9" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE10" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF10" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE11" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF11" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE12" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF12" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE13" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF13" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE14" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF14" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE15" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF15" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE16" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF16" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="17" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE17" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF17" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="18" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE18" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF18" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="19" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE19" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF19" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="20" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE20" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="21" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE21" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF21" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="22" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE22" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF22" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="23" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE23" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF23" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="24" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE24" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF24" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="25" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE25" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF25" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="26" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE26" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF26" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="27" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE27" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF27" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="28" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE28" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF28" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="29" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE29" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF29" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="30" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE30" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF30" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="31" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE31" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF31" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="32" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D32" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE32" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF32" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="33" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J33" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE33" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF33" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="34" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D34" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J34" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE34" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF34" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="35" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D35" s="7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J35" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE35" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF35" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="36" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D36" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="37" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J36" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE36" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF36" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="37" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D37" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J37" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE37" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF37" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="38" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D38" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="39" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J38" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE38" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF38" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="39" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D39" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="40" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J39" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE39" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF39" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="40" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D40" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="41" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J40" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE40" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF40" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="41" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D41" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="42" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J41" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE41" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF41" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="42" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D42" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="43" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J42" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE42" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF42" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="43" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D43" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="44" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J43" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE43" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF43" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="44" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D44" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J44" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE44" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF44" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="45" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D45" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="46" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J45" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE45" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF45" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="46" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D46" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="47" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J46" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE46" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF46" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="47" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D47" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="48" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J47" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE47" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF47" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="48" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D48" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J48" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE48" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF48" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="49" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D49" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="50" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J49" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE49" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF49" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="50" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D50" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="51" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J50" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE50" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF50" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="51" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D51" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="52" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J51" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE51" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF51" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="52" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D52" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="53" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J52" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE52" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF52" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="53" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D53" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="54" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J53" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE53" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF53" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="54" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D54" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="55" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J54" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE54" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF54" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="55" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D55" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="56" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J55" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE55" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF55" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="56" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D56" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="57" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J56" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE56" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF56" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="57" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D57" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="58" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J57" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE57" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF57" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="58" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D58" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="59" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J58" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE58" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF58" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="59" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D59" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="60" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J59" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE59" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF59" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="60" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D60" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="61" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J60" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE60" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF60" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="61" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D61" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="62" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J61" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE61" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF61" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="62" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D62" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="63" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J62" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE62" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF62" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="63" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D63" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="64" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J63" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE63" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF63" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="64" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D64" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="65" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J64" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE64" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF64" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="65" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D65" s="7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="66" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J65" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE65" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF65" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="66" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D66" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="67" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J66" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>::</v>
+      </c>
+      <c r="AE66" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF66" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="67" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D67" s="7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="68" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J67" s="10" t="str">
+        <f t="shared" ref="J67:J95" si="3">G67&amp;":"&amp;H67&amp;":"&amp;I67</f>
+        <v>::</v>
+      </c>
+      <c r="AE67" s="10" t="str">
+        <f t="shared" ref="AE67:AE95" si="4">L67&amp;": "&amp;M67</f>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF67" s="10" t="str">
+        <f t="shared" ref="AF67:AF95" si="5">TEXT(R67,"dd-")&amp;TEXT(Q67,"mmm-")&amp;TEXT(P67, "yyyy")</f>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="68" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D68" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="69" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J68" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE68" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF68" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="69" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D69" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="70" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J69" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE69" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF69" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="70" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D70" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="71" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J70" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE70" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF70" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="71" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D71" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="72" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J71" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE71" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF71" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="72" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D72" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="73" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J72" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE72" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF72" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="73" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D73" s="7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="74" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J73" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE73" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF73" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="74" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D74" s="7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="75" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J74" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE74" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF74" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="75" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D75" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="76" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J75" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE75" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF75" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="76" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D76" s="7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="77" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J76" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE76" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF76" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="77" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D77" s="7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="78" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J77" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE77" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF77" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="78" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D78" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="79" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J78" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE78" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF78" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="79" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D79" s="7" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="80" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J79" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE79" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF79" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="80" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D80" s="7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="81" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J80" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE80" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF80" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="81" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D81" s="7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="82" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J81" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE81" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF81" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="82" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D82" s="7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="83" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J82" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE82" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF82" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="83" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D83" s="7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="84" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J83" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE83" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF83" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="84" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D84" s="7" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="85" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J84" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE84" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF84" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="85" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D85" s="7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="86" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J85" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE85" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF85" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="86" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D86" s="7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="87" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J86" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE86" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF86" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="87" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D87" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="88" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J87" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE87" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF87" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="88" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D88" s="7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="89" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J88" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE88" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF88" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="89" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D89" s="7" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="90" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J89" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE89" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF89" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="90" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D90" s="7" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="91" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J90" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE90" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF90" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="91" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D91" s="7" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="92" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J91" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE91" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF91" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="92" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D92" s="7" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="93" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J92" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE92" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF92" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="93" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D93" s="7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="94" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J93" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE93" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF93" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="94" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D94" s="7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="95" spans="4:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J94" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE94" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF94" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="95" spans="4:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D95" s="7" t="s">
         <v>120</v>
       </c>
+      <c r="J95" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>::</v>
+      </c>
+      <c r="AE95" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="AF95" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>00-Jan-1900</v>
+      </c>
+    </row>
+    <row r="96" spans="4:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE96" s="12"/>
+      <c r="AF96" s="12"/>
+    </row>
+    <row r="97" spans="31:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE97" s="12"/>
+      <c r="AF97" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated fields and data format for months
Added columns for stateProvince and countyOrMunicipality. Month format
for date changed from digits to abbreviation, so changed the formula
that parses the date columns for GenBank upload.
</commit_message>
<xml_diff>
--- a/GGI Barcoding Specimen Spreadsheet.xlsx
+++ b/GGI Barcoding Specimen Spreadsheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DevineA\Documents\GitHub\GeneiousFIMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devinea/Documents/GitHub/GeneiousFIMS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="18276" windowHeight="10980"/>
+    <workbookView xWindow="1880" yWindow="2100" windowWidth="29460" windowHeight="16820"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,20 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>extractionPlateID</t>
   </si>
@@ -400,6 +408,12 @@
   </si>
   <si>
     <t>fieldNumber</t>
+  </si>
+  <si>
+    <t>stateProvince</t>
+  </si>
+  <si>
+    <t>countyOrMunicipality</t>
   </si>
 </sst>
 </file>
@@ -416,10 +430,12 @@
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -833,33 +849,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF97"/>
+  <dimension ref="A1:AH97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="19.5546875" customWidth="1"/>
-    <col min="17" max="17" width="17.88671875" customWidth="1"/>
-    <col min="30" max="30" width="14.44140625" style="5"/>
-    <col min="31" max="31" width="13.88671875" customWidth="1"/>
-    <col min="32" max="32" width="20.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" customWidth="1"/>
+    <col min="12" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="21.5" customWidth="1"/>
+    <col min="15" max="15" width="9.5" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.5" customWidth="1"/>
+    <col min="19" max="19" width="17.83203125" customWidth="1"/>
+    <col min="32" max="32" width="14.5" style="5"/>
+    <col min="33" max="33" width="13.83203125" customWidth="1"/>
+    <col min="34" max="34" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>124</v>
       </c>
@@ -896,68 +913,74 @@
       <c r="L1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="AA1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AB1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AC1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AD1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AE1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AF1" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
@@ -965,16 +988,16 @@
         <f>G2&amp;":"&amp;H2&amp;":"&amp;I2</f>
         <v>::</v>
       </c>
-      <c r="AE2" s="3" t="str">
-        <f>L2&amp;": "&amp;M2</f>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF2" s="3" t="e">
-        <f>TEXT(DATE(P2, Q2, R2), "dd-mmm-yyyy")</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG2" s="3" t="str">
+        <f>L2&amp;": "&amp;M2&amp;": "&amp;N2&amp;": "&amp;O2</f>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH2" s="3" t="str">
+        <f>TEXT(T2, "dd") &amp; "-" &amp; S2 &amp; "-" &amp; R2</f>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
@@ -982,16 +1005,16 @@
         <f t="shared" ref="J3:J66" si="0">G3&amp;":"&amp;H3&amp;":"&amp;I3</f>
         <v>::</v>
       </c>
-      <c r="AE3" s="3" t="str">
-        <f t="shared" ref="AE3:AE66" si="1">L3&amp;": "&amp;M3</f>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF3" s="3" t="e">
-        <f t="shared" ref="AF3:AF66" si="2">TEXT(DATE(P3, Q3, R3), "dd-mmm-yyyy")</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG3" s="3" t="str">
+        <f t="shared" ref="AG3:AG66" si="1">L3&amp;": "&amp;M3&amp;": "&amp;N3&amp;": "&amp;O3</f>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH3" s="3" t="str">
+        <f t="shared" ref="AH3:AH66" si="2">TEXT(T3, "dd") &amp; "-" &amp; S3 &amp; "-" &amp; R3</f>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
@@ -999,16 +1022,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF4" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG4" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH4" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1016,16 +1039,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF5" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH5" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1033,16 +1056,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF6" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH6" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1050,16 +1073,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE7" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF7" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH7" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1067,16 +1090,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE8" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF8" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH8" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1084,16 +1107,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE9" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF9" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH9" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
@@ -1101,16 +1124,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE10" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH10" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1118,16 +1141,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE11" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF11" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH11" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1135,16 +1158,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE12" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF12" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG12" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH12" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1152,16 +1175,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE13" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF13" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG13" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH13" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1169,16 +1192,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE14" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF14" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH14" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
@@ -1186,16 +1209,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE15" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF15" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH15" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1203,16 +1226,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE16" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF16" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="17" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG16" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH16" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="17" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1220,16 +1243,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE17" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF17" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG17" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH17" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="18" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1237,16 +1260,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE18" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF18" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="19" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG18" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH18" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="19" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
@@ -1254,16 +1277,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE19" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF19" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="20" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH19" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="20" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D20" s="1" t="s">
         <v>45</v>
       </c>
@@ -1271,16 +1294,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE20" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF20" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="21" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH20" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="21" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1288,16 +1311,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE21" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF21" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="22" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH21" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="22" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
@@ -1305,16 +1328,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE22" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF22" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="23" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH22" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="23" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D23" s="1" t="s">
         <v>48</v>
       </c>
@@ -1322,16 +1345,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF23" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="24" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH23" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="24" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1339,16 +1362,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF24" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="25" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH24" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="25" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D25" s="1" t="s">
         <v>50</v>
       </c>
@@ -1356,16 +1379,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF25" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="26" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH25" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="26" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D26" s="1" t="s">
         <v>51</v>
       </c>
@@ -1373,16 +1396,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE26" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF26" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="27" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH26" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="27" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D27" s="1" t="s">
         <v>52</v>
       </c>
@@ -1390,16 +1413,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF27" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="28" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH27" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="28" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D28" s="1" t="s">
         <v>53</v>
       </c>
@@ -1407,16 +1430,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE28" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF28" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="29" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG28" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH28" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="29" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D29" s="1" t="s">
         <v>54</v>
       </c>
@@ -1424,16 +1447,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE29" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF29" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="30" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH29" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="30" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D30" s="1" t="s">
         <v>55</v>
       </c>
@@ -1441,16 +1464,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE30" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF30" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="31" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG30" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH30" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="31" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D31" s="1" t="s">
         <v>56</v>
       </c>
@@ -1458,16 +1481,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE31" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF31" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="32" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG31" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH31" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="32" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D32" s="1" t="s">
         <v>57</v>
       </c>
@@ -1475,16 +1498,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF32" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="33" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG32" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="33" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D33" s="1" t="s">
         <v>58</v>
       </c>
@@ -1492,16 +1515,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE33" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF33" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="34" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="34" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D34" s="1" t="s">
         <v>59</v>
       </c>
@@ -1509,16 +1532,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE34" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF34" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="35" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG34" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH34" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="35" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D35" s="1" t="s">
         <v>60</v>
       </c>
@@ -1526,16 +1549,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF35" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="36" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG35" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH35" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="36" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D36" s="1" t="s">
         <v>61</v>
       </c>
@@ -1543,16 +1566,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF36" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="37" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG36" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH36" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="37" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D37" s="1" t="s">
         <v>62</v>
       </c>
@@ -1560,16 +1583,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE37" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF37" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="38" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG37" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH37" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="38" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D38" s="1" t="s">
         <v>63</v>
       </c>
@@ -1577,16 +1600,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE38" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF38" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="39" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG38" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH38" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="39" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D39" s="1" t="s">
         <v>64</v>
       </c>
@@ -1594,16 +1617,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE39" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF39" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="40" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH39" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="40" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D40" s="1" t="s">
         <v>65</v>
       </c>
@@ -1611,16 +1634,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE40" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF40" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="41" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG40" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH40" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="41" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D41" s="1" t="s">
         <v>66</v>
       </c>
@@ -1628,16 +1651,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE41" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF41" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="42" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG41" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH41" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="42" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="1" t="s">
         <v>67</v>
       </c>
@@ -1645,16 +1668,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE42" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF42" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="43" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG42" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH42" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="43" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D43" s="1" t="s">
         <v>68</v>
       </c>
@@ -1662,16 +1685,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE43" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF43" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="44" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG43" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH43" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="44" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D44" s="1" t="s">
         <v>69</v>
       </c>
@@ -1679,16 +1702,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE44" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF44" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="45" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG44" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH44" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="45" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D45" s="1" t="s">
         <v>70</v>
       </c>
@@ -1696,16 +1719,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE45" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF45" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="46" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG45" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH45" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="46" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D46" s="1" t="s">
         <v>71</v>
       </c>
@@ -1713,16 +1736,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE46" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF46" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="47" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG46" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH46" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="47" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D47" s="1" t="s">
         <v>72</v>
       </c>
@@ -1730,16 +1753,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE47" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF47" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="48" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG47" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH47" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="48" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="1" t="s">
         <v>73</v>
       </c>
@@ -1747,16 +1770,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF48" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="49" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG48" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH48" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="49" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D49" s="1" t="s">
         <v>74</v>
       </c>
@@ -1764,16 +1787,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF49" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="50" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH49" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="50" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D50" s="1" t="s">
         <v>75</v>
       </c>
@@ -1781,16 +1804,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE50" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF50" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="51" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG50" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH50" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="51" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D51" s="1" t="s">
         <v>76</v>
       </c>
@@ -1798,16 +1821,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE51" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF51" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="52" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG51" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH51" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="52" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D52" s="1" t="s">
         <v>77</v>
       </c>
@@ -1815,16 +1838,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE52" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF52" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="53" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG52" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH52" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="53" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D53" s="1" t="s">
         <v>78</v>
       </c>
@@ -1832,16 +1855,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE53" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF53" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="54" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG53" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH53" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="54" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D54" s="1" t="s">
         <v>79</v>
       </c>
@@ -1849,16 +1872,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE54" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF54" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="55" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG54" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH54" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="55" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D55" s="1" t="s">
         <v>80</v>
       </c>
@@ -1866,16 +1889,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE55" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF55" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="56" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG55" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH55" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="56" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D56" s="1" t="s">
         <v>81</v>
       </c>
@@ -1883,16 +1906,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE56" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF56" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="57" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG56" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH56" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="57" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D57" s="1" t="s">
         <v>82</v>
       </c>
@@ -1900,16 +1923,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE57" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF57" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="58" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG57" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH57" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="58" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D58" s="1" t="s">
         <v>83</v>
       </c>
@@ -1917,16 +1940,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE58" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF58" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="59" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG58" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH58" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="59" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D59" s="1" t="s">
         <v>84</v>
       </c>
@@ -1934,16 +1957,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE59" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF59" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="60" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG59" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH59" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="60" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D60" s="1" t="s">
         <v>85</v>
       </c>
@@ -1951,16 +1974,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE60" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF60" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="61" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG60" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH60" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="61" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D61" s="1" t="s">
         <v>86</v>
       </c>
@@ -1968,16 +1991,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE61" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF61" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="62" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG61" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH61" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="62" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D62" s="1" t="s">
         <v>87</v>
       </c>
@@ -1985,16 +2008,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE62" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF62" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="63" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG62" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH62" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="63" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D63" s="1" t="s">
         <v>88</v>
       </c>
@@ -2002,16 +2025,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE63" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF63" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="64" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG63" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH63" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="64" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D64" s="1" t="s">
         <v>89</v>
       </c>
@@ -2019,16 +2042,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE64" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF64" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="65" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG64" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH64" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="65" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D65" s="1" t="s">
         <v>90</v>
       </c>
@@ -2036,16 +2059,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE65" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF65" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="66" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG65" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH65" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="66" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D66" s="1" t="s">
         <v>91</v>
       </c>
@@ -2053,16 +2076,16 @@
         <f t="shared" si="0"/>
         <v>::</v>
       </c>
-      <c r="AE66" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF66" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="67" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG66" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH66" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="67" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D67" s="1" t="s">
         <v>92</v>
       </c>
@@ -2070,16 +2093,16 @@
         <f t="shared" ref="J67:J95" si="3">G67&amp;":"&amp;H67&amp;":"&amp;I67</f>
         <v>::</v>
       </c>
-      <c r="AE67" s="3" t="str">
-        <f t="shared" ref="AE67:AE95" si="4">L67&amp;": "&amp;M67</f>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF67" s="3" t="e">
-        <f t="shared" ref="AF67:AF95" si="5">TEXT(DATE(P67, Q67, R67), "dd-mmm-yyyy")</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="68" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG67" s="3" t="str">
+        <f t="shared" ref="AG67:AG95" si="4">L67&amp;": "&amp;M67&amp;": "&amp;N67&amp;": "&amp;O67</f>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH67" s="3" t="str">
+        <f t="shared" ref="AH67:AH95" si="5">TEXT(T67, "dd") &amp; "-" &amp; S67 &amp; "-" &amp; R67</f>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="68" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D68" s="1" t="s">
         <v>93</v>
       </c>
@@ -2087,16 +2110,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE68" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF68" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="69" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG68" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH68" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="69" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D69" s="1" t="s">
         <v>94</v>
       </c>
@@ -2104,16 +2127,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE69" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF69" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="70" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG69" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH69" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="70" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D70" s="1" t="s">
         <v>95</v>
       </c>
@@ -2121,16 +2144,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE70" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF70" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="71" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG70" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH70" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="71" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D71" s="1" t="s">
         <v>96</v>
       </c>
@@ -2138,16 +2161,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE71" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF71" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="72" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG71" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH71" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="72" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D72" s="1" t="s">
         <v>97</v>
       </c>
@@ -2155,16 +2178,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE72" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF72" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="73" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG72" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH72" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="73" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D73" s="1" t="s">
         <v>98</v>
       </c>
@@ -2172,16 +2195,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE73" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF73" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="74" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG73" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH73" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="74" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D74" s="1" t="s">
         <v>99</v>
       </c>
@@ -2189,16 +2212,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE74" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF74" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="75" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG74" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH74" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="75" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D75" s="1" t="s">
         <v>100</v>
       </c>
@@ -2206,16 +2229,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE75" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF75" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="76" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG75" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH75" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="76" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D76" s="1" t="s">
         <v>101</v>
       </c>
@@ -2223,16 +2246,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE76" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF76" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="77" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG76" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH76" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="77" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D77" s="1" t="s">
         <v>102</v>
       </c>
@@ -2240,16 +2263,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE77" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF77" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="78" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG77" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH77" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="78" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D78" s="1" t="s">
         <v>103</v>
       </c>
@@ -2257,16 +2280,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE78" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF78" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="79" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG78" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH78" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="79" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D79" s="1" t="s">
         <v>104</v>
       </c>
@@ -2274,16 +2297,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE79" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF79" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="80" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG79" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH79" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="80" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D80" s="1" t="s">
         <v>105</v>
       </c>
@@ -2291,16 +2314,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE80" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF80" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="81" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG80" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH80" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="81" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D81" s="1" t="s">
         <v>106</v>
       </c>
@@ -2308,16 +2331,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE81" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF81" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="82" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG81" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH81" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="82" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D82" s="1" t="s">
         <v>107</v>
       </c>
@@ -2325,16 +2348,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE82" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF82" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="83" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG82" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH82" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="83" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D83" s="1" t="s">
         <v>108</v>
       </c>
@@ -2342,16 +2365,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE83" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF83" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="84" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG83" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH83" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="84" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D84" s="1" t="s">
         <v>109</v>
       </c>
@@ -2359,16 +2382,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE84" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF84" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="85" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG84" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH84" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="85" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D85" s="1" t="s">
         <v>110</v>
       </c>
@@ -2376,16 +2399,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE85" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF85" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="86" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG85" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH85" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="86" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D86" s="1" t="s">
         <v>111</v>
       </c>
@@ -2393,16 +2416,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE86" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF86" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="87" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG86" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH86" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="87" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D87" s="1" t="s">
         <v>112</v>
       </c>
@@ -2410,16 +2433,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE87" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF87" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="88" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG87" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH87" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="88" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D88" s="1" t="s">
         <v>113</v>
       </c>
@@ -2427,16 +2450,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE88" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF88" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="89" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG88" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH88" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="89" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D89" s="1" t="s">
         <v>114</v>
       </c>
@@ -2444,16 +2467,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE89" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF89" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="90" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG89" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH89" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="90" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D90" s="1" t="s">
         <v>115</v>
       </c>
@@ -2461,16 +2484,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE90" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF90" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="91" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG90" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH90" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="91" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D91" s="1" t="s">
         <v>116</v>
       </c>
@@ -2478,16 +2501,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE91" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF91" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="92" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG91" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH91" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="92" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D92" s="1" t="s">
         <v>117</v>
       </c>
@@ -2495,16 +2518,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE92" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF92" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="93" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG92" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH92" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="93" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D93" s="1" t="s">
         <v>118</v>
       </c>
@@ -2512,16 +2535,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE93" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF93" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="94" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG93" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH93" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="94" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D94" s="1" t="s">
         <v>119</v>
       </c>
@@ -2529,16 +2552,16 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE94" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF94" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="95" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG94" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH94" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="95" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D95" s="1" t="s">
         <v>120</v>
       </c>
@@ -2546,22 +2569,22 @@
         <f t="shared" si="3"/>
         <v>::</v>
       </c>
-      <c r="AE95" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">: </v>
-      </c>
-      <c r="AF95" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="96" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AE96" s="5"/>
-      <c r="AF96" s="5"/>
-    </row>
-    <row r="97" spans="31:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AE97" s="5"/>
-      <c r="AF97" s="5"/>
+      <c r="AG95" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">: : : </v>
+      </c>
+      <c r="AH95" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00--</v>
+      </c>
+    </row>
+    <row r="96" spans="4:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AG96" s="5"/>
+      <c r="AH96" s="5"/>
+    </row>
+    <row r="97" spans="33:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AG97" s="5"/>
+      <c r="AH97" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>